<commit_message>
@ ntw push bugs
</commit_message>
<xml_diff>
--- a/0-docs/entreprenariat/Planning-TODO-LIST-INNOV-PROJECT.xlsx
+++ b/0-docs/entreprenariat/Planning-TODO-LIST-INNOV-PROJECT.xlsx
@@ -4,21 +4,23 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="NOYAU" sheetId="1" r:id="rId1"/>
-    <sheet name="ERP-SCOOLAIRE" sheetId="2" r:id="rId2"/>
-    <sheet name="Gestion Commercial" sheetId="3" r:id="rId3"/>
-    <sheet name="RH&amp;PAIE" sheetId="4" r:id="rId4"/>
-    <sheet name="centre de santé" sheetId="5" r:id="rId5"/>
+    <sheet name="Feuil1" sheetId="6" r:id="rId2"/>
+    <sheet name="ERP-SCOOLAIRE" sheetId="2" r:id="rId3"/>
+    <sheet name="Gestion Commercial" sheetId="3" r:id="rId4"/>
+    <sheet name="RH&amp;PAIE" sheetId="4" r:id="rId5"/>
+    <sheet name="centre de santé" sheetId="5" r:id="rId6"/>
+    <sheet name="Bugs Noyau" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="34">
   <si>
     <t>Activité</t>
   </si>
@@ -93,6 +95,33 @@
   </si>
   <si>
     <t>Manuel Utilisateur</t>
+  </si>
+  <si>
+    <t>BUGS</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Bugs</t>
+  </si>
+  <si>
+    <t>Après l'affichage d'un etat le clic sur le bouton quitter genére un erreur</t>
+  </si>
+  <si>
+    <t>Pas bloquant</t>
+  </si>
+  <si>
+    <t>Bloquant</t>
+  </si>
+  <si>
+    <t>Impossible d'affiche un modal panel secondaire a partir d'un modal primaire (3eme modal)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garder le focus sur le menu et le menu-item </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rechecher  avec seachkey nepasse pas </t>
   </si>
 </sst>
 </file>
@@ -116,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,6 +155,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -157,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -172,12 +207,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -499,14 +540,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="2"/>
@@ -598,6 +639,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F10"/>
   <sheetViews>
@@ -613,14 +666,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -649,10 +702,10 @@
       <c r="B4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>43472</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>43479</v>
       </c>
       <c r="E4" s="6" t="s">
@@ -665,13 +718,13 @@
         <f>A4+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>43476</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>43476</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -687,10 +740,10 @@
       <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>43477</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>43477</v>
       </c>
       <c r="E6" s="6" t="s">
@@ -706,10 +759,10 @@
       <c r="B7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>43474</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>43481</v>
       </c>
       <c r="E7" s="6" t="s">
@@ -725,10 +778,10 @@
       <c r="B8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>43482</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>43492</v>
       </c>
       <c r="E8" s="6" t="s">
@@ -742,8 +795,8 @@
         <v>6</v>
       </c>
       <c r="B9" s="7"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="6"/>
       <c r="F9" s="7"/>
     </row>
@@ -753,7 +806,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="10"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="7"/>
       <c r="E10" s="6"/>
       <c r="F10" s="7"/>
@@ -766,7 +819,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F7"/>
   <sheetViews>
@@ -782,14 +835,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -830,11 +883,11 @@
         <f>A4+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
       <c r="E5" s="6" t="s">
         <v>7</v>
       </c>
@@ -870,7 +923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F7"/>
   <sheetViews>
@@ -885,14 +938,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -933,9 +986,9 @@
         <f>A4+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
       <c r="E5" s="6"/>
       <c r="F5" s="7"/>
     </row>
@@ -969,7 +1022,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F7"/>
   <sheetViews>
@@ -985,14 +1038,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1021,10 +1074,10 @@
       <c r="B4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>43474</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>43481</v>
       </c>
       <c r="E4" s="6" t="s">
@@ -1037,13 +1090,13 @@
         <f>A4+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>43482</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>43493</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -1079,4 +1132,97 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="82.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>43473</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>43473</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>43473</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>43473</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
mise a jour BKD 14/01/2019
</commit_message>
<xml_diff>
--- a/0-docs/entreprenariat/Planning-TODO-LIST-INNOV-PROJECT.xlsx
+++ b/0-docs/entreprenariat/Planning-TODO-LIST-INNOV-PROJECT.xlsx
@@ -145,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +161,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -192,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -210,15 +216,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,14 +550,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="2"/>
@@ -666,14 +676,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -835,14 +845,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -938,14 +948,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1038,14 +1048,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1139,7 +1149,7 @@
   <dimension ref="A2:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B14" sqref="B14:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,11 +1160,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1175,7 +1185,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+      <c r="A4" s="11">
         <v>43473</v>
       </c>
       <c r="B4" t="s">
@@ -1186,7 +1196,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+      <c r="A5" s="11">
         <v>43473</v>
       </c>
       <c r="B5" t="s">
@@ -1196,19 +1206,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
+    <row r="6" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
         <v>43473</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="A7" s="11">
         <v>43473</v>
       </c>
       <c r="B7" t="s">

</xml_diff>